<commit_message>
Almost finished chem IA
</commit_message>
<xml_diff>
--- a/Physics/draft/light.xlsx
+++ b/Physics/draft/light.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder2021\IAProjects\Physics\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EA3FD4-15B3-4A45-BFE6-08E9248560C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF2E6B-C14C-4A12-8F08-DF1217C6FC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="14640" windowHeight="22680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Averaging</t>
   </si>
   <si>
-    <t>Half Range (lux)</t>
-  </si>
-  <si>
     <t>Absolute Error (lux)</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Distance % Error</t>
   </si>
   <si>
-    <t>Average Illuminance (lux)</t>
-  </si>
-  <si>
     <t>Graph</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t xml:space="preserve">1/Distance^2 </t>
+  </si>
+  <si>
+    <t>Average Illuminance (lx)</t>
+  </si>
+  <si>
+    <t>Half Range (lx)</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1025,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Average Illuminance (lux)</c:v>
+                  <c:v>Average Illuminance (lx)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4609,8 +4609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="6" spans="3:8">
       <c r="D6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="19" spans="3:8">
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -4843,12 +4843,12 @@
     </row>
     <row r="22" spans="3:8">
       <c r="C22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="3:8">
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
         <f>D17*D18</f>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="25" spans="3:8">
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25">
         <f>0.01/D17</f>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="26" spans="3:8">
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <f>0.01/D18</f>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="27" spans="3:8">
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <f>D25+D26</f>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="28" spans="3:8">
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1">
         <f>D24*D27</f>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="35" spans="3:8">
       <c r="C35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -5135,21 +5135,21 @@
     </row>
     <row r="50" spans="3:6">
       <c r="D50" s="9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="3:6" ht="15">
       <c r="C51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" t="s">
+        <v>43</v>
+      </c>
+      <c r="F51" t="s">
         <v>20</v>
-      </c>
-      <c r="F51" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="52" spans="3:6">
@@ -5298,25 +5298,25 @@
     </row>
     <row r="79" spans="3:3">
       <c r="C79" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="3:12" ht="14.25" customHeight="1">
       <c r="C81" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F81" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G81" t="str">
         <f>D50</f>
-        <v>Average Illuminance (lux)</v>
+        <v>Average Illuminance (lx)</v>
       </c>
     </row>
     <row r="82" spans="3:12">
@@ -5593,7 +5593,7 @@
     </row>
     <row r="92" spans="3:12">
       <c r="C92" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D92">
         <v>1111.1111111111111</v>
@@ -5622,7 +5622,7 @@
     </row>
     <row r="93" spans="3:12">
       <c r="C93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D93">
         <v>3.3333333333333333E-2</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="94" spans="3:12">
       <c r="C94" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D94">
         <v>6.6666666666666666E-2</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="95" spans="3:12">
       <c r="C95" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D95">
         <v>74.074074074074076</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="97" spans="3:6">
       <c r="C97" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="3:6">
@@ -5719,13 +5719,13 @@
       </c>
       <c r="D100" t="str">
         <f>D50</f>
-        <v>Average Illuminance (lux)</v>
+        <v>Average Illuminance (lx)</v>
       </c>
       <c r="E100" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F100" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="3:6">

</xml_diff>

<commit_message>
Changed some english stuff
</commit_message>
<xml_diff>
--- a/Physics/draft/light.xlsx
+++ b/Physics/draft/light.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Folder2021\IAProjects\Physics\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FF2E6B-C14C-4A12-8F08-DF1217C6FC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CD29DA-C377-4B27-A2E1-59D5CA6F4DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>Averaging</t>
   </si>
   <si>
-    <t>Absolute Error (lux)</t>
-  </si>
-  <si>
     <r>
       <t>Distance (</t>
     </r>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Half Range (lx)</t>
+  </si>
+  <si>
+    <t>Absolute Error (lx)</t>
   </si>
 </sst>
 </file>
@@ -4609,8 +4609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="6" spans="3:8">
       <c r="D6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -4835,7 +4835,7 @@
     </row>
     <row r="19" spans="3:8">
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -4843,12 +4843,12 @@
     </row>
     <row r="22" spans="3:8">
       <c r="C22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="3:8">
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24">
         <f>D17*D18</f>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="25" spans="3:8">
       <c r="C25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25">
         <f>0.01/D17</f>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="26" spans="3:8">
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26">
         <f>0.01/D18</f>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="27" spans="3:8">
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27">
         <f>D25+D26</f>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="28" spans="3:8">
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1">
         <f>D24*D27</f>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="35" spans="3:8">
       <c r="C35" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -5135,21 +5135,21 @@
     </row>
     <row r="50" spans="3:6">
       <c r="D50" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
     <row r="51" spans="3:6" ht="15">
       <c r="C51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" t="s">
         <v>43</v>
-      </c>
-      <c r="F51" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="52" spans="3:6">
@@ -5298,21 +5298,21 @@
     </row>
     <row r="79" spans="3:3">
       <c r="C79" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="3:12" ht="14.25" customHeight="1">
       <c r="C81" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E81" t="s">
+        <v>33</v>
+      </c>
+      <c r="F81" t="s">
         <v>34</v>
-      </c>
-      <c r="F81" t="s">
-        <v>35</v>
       </c>
       <c r="G81" t="str">
         <f>D50</f>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="92" spans="3:12">
       <c r="C92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D92">
         <v>1111.1111111111111</v>
@@ -5622,7 +5622,7 @@
     </row>
     <row r="93" spans="3:12">
       <c r="C93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D93">
         <v>3.3333333333333333E-2</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="94" spans="3:12">
       <c r="C94" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D94">
         <v>6.6666666666666666E-2</v>
@@ -5680,7 +5680,7 @@
     </row>
     <row r="95" spans="3:12">
       <c r="C95" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D95">
         <v>74.074074074074076</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="97" spans="3:6">
       <c r="C97" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="3:6">
@@ -5722,10 +5722,10 @@
         <v>Average Illuminance (lx)</v>
       </c>
       <c r="E100" t="s">
+        <v>38</v>
+      </c>
+      <c r="F100" t="s">
         <v>39</v>
-      </c>
-      <c r="F100" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="101" spans="3:6">

</xml_diff>